<commit_message>
+ Default Market Settings
</commit_message>
<xml_diff>
--- a/documentation/images/ItemImbalance.xlsx
+++ b/documentation/images/ItemImbalance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumente\Minecraft\mods\StockMarket\MC_1.20.1_StockMarket\documentation\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39E96DFE-A01B-453C-9DEE-3D9B47FF1CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1D0756-7FFD-4E42-AEC0-733CBACA068D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8C28FF7D-EFDF-481B-87CE-C7A9ADAE27D1}"/>
+    <workbookView minimized="1" xWindow="41400" yWindow="9270" windowWidth="24375" windowHeight="11160" xr2:uid="{8C28FF7D-EFDF-481B-87CE-C7A9ADAE27D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>